<commit_message>
1.computer the hs300 for new sample
</commit_message>
<xml_diff>
--- a/300inout.xlsx
+++ b/300inout.xlsx
@@ -11,14 +11,14 @@
     <sheet name="20080630" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">data!$A$1:$D$1973</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">data!$A$1:$D$1991</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10451" uniqueCount="2000">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10542" uniqueCount="2012">
   <si>
     <t>变更日期</t>
   </si>
@@ -6047,6 +6047,42 @@
   </si>
   <si>
     <t>晶科能源</t>
+  </si>
+  <si>
+    <t>2023-12-11</t>
+  </si>
+  <si>
+    <t>中际旭创</t>
+  </si>
+  <si>
+    <t>华大九天</t>
+  </si>
+  <si>
+    <t>中航机载</t>
+  </si>
+  <si>
+    <t>海南机场</t>
+  </si>
+  <si>
+    <t>中国海油</t>
+  </si>
+  <si>
+    <t>信达证券</t>
+  </si>
+  <si>
+    <t>海光信息</t>
+  </si>
+  <si>
+    <t>寒武纪-U</t>
+  </si>
+  <si>
+    <t>联影医疗</t>
+  </si>
+  <si>
+    <t>君正集团</t>
+  </si>
+  <si>
+    <t>弘元绿能</t>
   </si>
 </sst>
 </file>
@@ -6673,7 +6709,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -6688,9 +6724,17 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" quotePrefix="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" quotePrefix="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -7039,12 +7083,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D1991"/>
+  <dimension ref="A1:D2019"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1973" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2000" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="B1983" sqref="B1983:B1991"/>
+      <selection pane="bottomLeft" activeCell="D2005" sqref="D2005"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="3"/>
@@ -34259,7 +34303,7 @@
       <c r="A1944" s="4" t="s">
         <v>1982</v>
       </c>
-      <c r="B1944" s="6" t="s">
+      <c r="B1944" s="8" t="s">
         <v>1587</v>
       </c>
       <c r="C1944" s="3" t="s">
@@ -34273,7 +34317,7 @@
       <c r="A1945" s="4" t="s">
         <v>1982</v>
       </c>
-      <c r="B1945" s="6" t="s">
+      <c r="B1945" s="8" t="s">
         <v>154</v>
       </c>
       <c r="C1945" s="3" t="s">
@@ -34287,7 +34331,7 @@
       <c r="A1946" s="4" t="s">
         <v>1982</v>
       </c>
-      <c r="B1946" s="6" t="s">
+      <c r="B1946" s="8" t="s">
         <v>1983</v>
       </c>
       <c r="C1946" s="3" t="s">
@@ -34301,7 +34345,7 @@
       <c r="A1947" s="4" t="s">
         <v>1982</v>
       </c>
-      <c r="B1947" s="6" t="s">
+      <c r="B1947" s="8" t="s">
         <v>1985</v>
       </c>
       <c r="C1947" s="3" t="s">
@@ -34469,7 +34513,7 @@
       <c r="A1959" s="4" t="s">
         <v>1982</v>
       </c>
-      <c r="B1959" s="6" t="s">
+      <c r="B1959" s="8" t="s">
         <v>38</v>
       </c>
       <c r="C1959" s="3" t="s">
@@ -34483,7 +34527,7 @@
       <c r="A1960" s="4" t="s">
         <v>1982</v>
       </c>
-      <c r="B1960" s="6" t="s">
+      <c r="B1960" s="8" t="s">
         <v>1216</v>
       </c>
       <c r="C1960" s="3" t="s">
@@ -34497,7 +34541,7 @@
       <c r="A1961" s="4" t="s">
         <v>1982</v>
       </c>
-      <c r="B1961" s="6" t="s">
+      <c r="B1961" s="8" t="s">
         <v>1463</v>
       </c>
       <c r="C1961" s="3" t="s">
@@ -34511,7 +34555,7 @@
       <c r="A1962" s="4" t="s">
         <v>1982</v>
       </c>
-      <c r="B1962" s="6" t="s">
+      <c r="B1962" s="8" t="s">
         <v>1734</v>
       </c>
       <c r="C1962" s="3" t="s">
@@ -34525,7 +34569,7 @@
       <c r="A1963" s="4" t="s">
         <v>1982</v>
       </c>
-      <c r="B1963" s="6" t="s">
+      <c r="B1963" s="8" t="s">
         <v>1897</v>
       </c>
       <c r="C1963" s="3" t="s">
@@ -34679,7 +34723,7 @@
       <c r="A1974" s="4" t="s">
         <v>1995</v>
       </c>
-      <c r="B1974" s="6" t="s">
+      <c r="B1974" s="8" t="s">
         <v>674</v>
       </c>
       <c r="C1974" s="3" t="s">
@@ -34693,7 +34737,7 @@
       <c r="A1975" s="4" t="s">
         <v>1995</v>
       </c>
-      <c r="B1975" s="6" t="s">
+      <c r="B1975" s="8" t="s">
         <v>246</v>
       </c>
       <c r="C1975" t="s">
@@ -34805,7 +34849,7 @@
       <c r="A1983" s="4" t="s">
         <v>1995</v>
       </c>
-      <c r="B1983" s="6" t="s">
+      <c r="B1983" s="8" t="s">
         <v>748</v>
       </c>
       <c r="C1983" t="s">
@@ -34819,7 +34863,7 @@
       <c r="A1984" s="4" t="s">
         <v>1995</v>
       </c>
-      <c r="B1984" s="6" t="s">
+      <c r="B1984" s="8" t="s">
         <v>1669</v>
       </c>
       <c r="C1984" t="s">
@@ -34833,7 +34877,7 @@
       <c r="A1985" s="4" t="s">
         <v>1995</v>
       </c>
-      <c r="B1985" s="6" t="s">
+      <c r="B1985" s="8" t="s">
         <v>1806</v>
       </c>
       <c r="C1985" t="s">
@@ -34847,7 +34891,7 @@
       <c r="A1986" s="4" t="s">
         <v>1995</v>
       </c>
-      <c r="B1986" s="6" t="s">
+      <c r="B1986" s="8" t="s">
         <v>1544</v>
       </c>
       <c r="C1986" t="s">
@@ -34927,9 +34971,401 @@
         <v>607</v>
       </c>
     </row>
+    <row r="1992" spans="1:4">
+      <c r="A1992" s="4" t="s">
+        <v>2000</v>
+      </c>
+      <c r="B1992" s="9" t="s">
+        <v>992</v>
+      </c>
+      <c r="C1992" t="s">
+        <v>1494</v>
+      </c>
+      <c r="D1992" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1993" spans="1:4">
+      <c r="A1993" s="4" t="s">
+        <v>2000</v>
+      </c>
+      <c r="B1993" s="10" t="s">
+        <v>1193</v>
+      </c>
+      <c r="C1993" t="s">
+        <v>1194</v>
+      </c>
+      <c r="D1993" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1994" spans="1:4">
+      <c r="A1994" s="4" t="s">
+        <v>2000</v>
+      </c>
+      <c r="B1994" s="7">
+        <v>300308</v>
+      </c>
+      <c r="C1994" t="s">
+        <v>2001</v>
+      </c>
+      <c r="D1994" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1995" spans="1:4">
+      <c r="A1995" s="4" t="s">
+        <v>2000</v>
+      </c>
+      <c r="B1995" s="7">
+        <v>301269</v>
+      </c>
+      <c r="C1995" t="s">
+        <v>2002</v>
+      </c>
+      <c r="D1995" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1996" spans="1:4">
+      <c r="A1996" s="4" t="s">
+        <v>2000</v>
+      </c>
+      <c r="B1996" s="7">
+        <v>600023</v>
+      </c>
+      <c r="C1996" t="s">
+        <v>1336</v>
+      </c>
+      <c r="D1996" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1997" spans="1:4">
+      <c r="A1997" s="4" t="s">
+        <v>2000</v>
+      </c>
+      <c r="B1997" s="7">
+        <v>600372</v>
+      </c>
+      <c r="C1997" t="s">
+        <v>2003</v>
+      </c>
+      <c r="D1997" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1998" spans="1:4">
+      <c r="A1998" s="4" t="s">
+        <v>2000</v>
+      </c>
+      <c r="B1998" s="7">
+        <v>600489</v>
+      </c>
+      <c r="C1998" t="s">
+        <v>439</v>
+      </c>
+      <c r="D1998" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1999" spans="1:4">
+      <c r="A1999" s="4" t="s">
+        <v>2000</v>
+      </c>
+      <c r="B1999" s="7">
+        <v>600515</v>
+      </c>
+      <c r="C1999" t="s">
+        <v>2004</v>
+      </c>
+      <c r="D1999" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2000" spans="1:4">
+      <c r="A2000" s="4" t="s">
+        <v>2000</v>
+      </c>
+      <c r="B2000" s="7">
+        <v>600938</v>
+      </c>
+      <c r="C2000" t="s">
+        <v>2005</v>
+      </c>
+      <c r="D2000" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2001" spans="1:4">
+      <c r="A2001" s="4" t="s">
+        <v>2000</v>
+      </c>
+      <c r="B2001" s="7">
+        <v>601059</v>
+      </c>
+      <c r="C2001" t="s">
+        <v>2006</v>
+      </c>
+      <c r="D2001" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2002" spans="1:4">
+      <c r="A2002" s="4" t="s">
+        <v>2000</v>
+      </c>
+      <c r="B2002" s="7">
+        <v>601916</v>
+      </c>
+      <c r="C2002" t="s">
+        <v>1794</v>
+      </c>
+      <c r="D2002" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2003" spans="1:4">
+      <c r="A2003" s="4" t="s">
+        <v>2000</v>
+      </c>
+      <c r="B2003" s="7">
+        <v>688041</v>
+      </c>
+      <c r="C2003" t="s">
+        <v>2007</v>
+      </c>
+      <c r="D2003" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2004" spans="1:4">
+      <c r="A2004" s="4" t="s">
+        <v>2000</v>
+      </c>
+      <c r="B2004" s="7">
+        <v>688256</v>
+      </c>
+      <c r="C2004" t="s">
+        <v>2008</v>
+      </c>
+      <c r="D2004" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2005" spans="1:4">
+      <c r="A2005" s="4" t="s">
+        <v>2000</v>
+      </c>
+      <c r="B2005" s="7">
+        <v>688271</v>
+      </c>
+      <c r="C2005" t="s">
+        <v>2009</v>
+      </c>
+      <c r="D2005" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2006" spans="1:4">
+      <c r="A2006" s="4" t="s">
+        <v>2000</v>
+      </c>
+      <c r="B2006" s="10" t="s">
+        <v>1587</v>
+      </c>
+      <c r="C2006" t="s">
+        <v>1588</v>
+      </c>
+      <c r="D2006" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="2007" spans="1:4">
+      <c r="A2007" s="4" t="s">
+        <v>2000</v>
+      </c>
+      <c r="B2007" s="10" t="s">
+        <v>1890</v>
+      </c>
+      <c r="C2007" t="s">
+        <v>1891</v>
+      </c>
+      <c r="D2007" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="2008" spans="1:4">
+      <c r="A2008" s="4" t="s">
+        <v>2000</v>
+      </c>
+      <c r="B2008" s="10" t="s">
+        <v>1671</v>
+      </c>
+      <c r="C2008" t="s">
+        <v>1672</v>
+      </c>
+      <c r="D2008" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="2009" spans="1:4">
+      <c r="A2009" s="4" t="s">
+        <v>2000</v>
+      </c>
+      <c r="B2009" s="10" t="s">
+        <v>1804</v>
+      </c>
+      <c r="C2009" t="s">
+        <v>1805</v>
+      </c>
+      <c r="D2009" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="2010" spans="1:4">
+      <c r="A2010" s="4" t="s">
+        <v>2000</v>
+      </c>
+      <c r="B2010" s="10" t="s">
+        <v>1985</v>
+      </c>
+      <c r="C2010" t="s">
+        <v>1986</v>
+      </c>
+      <c r="D2010" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="2011" spans="1:4">
+      <c r="A2011" s="4" t="s">
+        <v>2000</v>
+      </c>
+      <c r="B2011" s="7">
+        <v>300207</v>
+      </c>
+      <c r="C2011" t="s">
+        <v>1948</v>
+      </c>
+      <c r="D2011" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="2012" spans="1:4">
+      <c r="A2012" s="4" t="s">
+        <v>2000</v>
+      </c>
+      <c r="B2012" s="7">
+        <v>300601</v>
+      </c>
+      <c r="C2012" t="s">
+        <v>1777</v>
+      </c>
+      <c r="D2012" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="2013" spans="1:4">
+      <c r="A2013" s="4" t="s">
+        <v>2000</v>
+      </c>
+      <c r="B2013" s="7">
+        <v>300769</v>
+      </c>
+      <c r="C2013" t="s">
+        <v>1987</v>
+      </c>
+      <c r="D2013" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="2014" spans="1:4">
+      <c r="A2014" s="4" t="s">
+        <v>2000</v>
+      </c>
+      <c r="B2014" s="7">
+        <v>600383</v>
+      </c>
+      <c r="C2014" t="s">
+        <v>658</v>
+      </c>
+      <c r="D2014" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="2015" spans="1:4">
+      <c r="A2015" s="4" t="s">
+        <v>2000</v>
+      </c>
+      <c r="B2015" s="7">
+        <v>600763</v>
+      </c>
+      <c r="C2015" t="s">
+        <v>1821</v>
+      </c>
+      <c r="D2015" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="2016" spans="1:4">
+      <c r="A2016" s="4" t="s">
+        <v>2000</v>
+      </c>
+      <c r="B2016" s="7">
+        <v>600884</v>
+      </c>
+      <c r="C2016" t="s">
+        <v>593</v>
+      </c>
+      <c r="D2016" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="2017" spans="1:4">
+      <c r="A2017" s="4" t="s">
+        <v>2000</v>
+      </c>
+      <c r="B2017" s="7">
+        <v>601216</v>
+      </c>
+      <c r="C2017" t="s">
+        <v>2010</v>
+      </c>
+      <c r="D2017" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="2018" spans="1:4">
+      <c r="A2018" s="4" t="s">
+        <v>2000</v>
+      </c>
+      <c r="B2018" s="7">
+        <v>603185</v>
+      </c>
+      <c r="C2018" t="s">
+        <v>2011</v>
+      </c>
+      <c r="D2018" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="2019" spans="1:4">
+      <c r="A2019" s="4" t="s">
+        <v>2000</v>
+      </c>
+      <c r="B2019" s="7">
+        <v>688005</v>
+      </c>
+      <c r="C2019" t="s">
+        <v>1977</v>
+      </c>
+      <c r="D2019" t="s">
+        <v>607</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:D1973">
-    <sortState ref="A1:D1973">
+  <autoFilter ref="A1:D1991">
+    <sortState ref="A1:D1991">
       <sortCondition ref="A2"/>
     </sortState>
     <extLst/>
@@ -34938,7 +35374,7 @@
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter/>
   <ignoredErrors>
-    <ignoredError sqref="B1983:B1986 B1974:B1975" numberStoredAsText="1"/>
+    <ignoredError sqref="B2006:B2010 B1992:B1993 B1974:B1975 B1983:B1986" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
1.get_fin_date for different datetime 2.add proxy for datascatter 3.update 300inout
</commit_message>
<xml_diff>
--- a/300inout.xlsx
+++ b/300inout.xlsx
@@ -11,7 +11,7 @@
     <sheet name="20080630" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">data!$A$1:$D$2019</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">data!$A$1:$D$2043</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10619" uniqueCount="2020">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10731" uniqueCount="2032">
   <si>
     <t>变更日期</t>
   </si>
@@ -6120,6 +6120,42 @@
   </si>
   <si>
     <t>华侨城 A</t>
+  </si>
+  <si>
+    <t>2024-12-13</t>
+  </si>
+  <si>
+    <t>山金国际</t>
+  </si>
+  <si>
+    <t>天孚通信</t>
+  </si>
+  <si>
+    <t>新易盛</t>
+  </si>
+  <si>
+    <t>赛力斯</t>
+  </si>
+  <si>
+    <t>首创证券</t>
+  </si>
+  <si>
+    <t>阿特斯</t>
+  </si>
+  <si>
+    <t>百利天恒</t>
+  </si>
+  <si>
+    <t>晨光股份</t>
+  </si>
+  <si>
+    <t>2025-02-06</t>
+  </si>
+  <si>
+    <t>赛轮轮胎</t>
+  </si>
+  <si>
+    <t>海通证券</t>
   </si>
 </sst>
 </file>
@@ -7121,12 +7157,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D2043"/>
+  <dimension ref="A1:D2077"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2026" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2061" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="D2031" sqref="D2031"/>
+      <selection pane="bottomLeft" activeCell="B2076" sqref="B2076"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="3"/>
@@ -35737,9 +35773,485 @@
         <v>607</v>
       </c>
     </row>
+    <row r="2044" spans="1:4">
+      <c r="A2044" s="4" t="s">
+        <v>2020</v>
+      </c>
+      <c r="B2044" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="C2044" t="s">
+        <v>1761</v>
+      </c>
+      <c r="D2044" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2045" spans="1:4">
+      <c r="A2045" s="4" t="s">
+        <v>2020</v>
+      </c>
+      <c r="B2045" s="11" t="s">
+        <v>618</v>
+      </c>
+      <c r="C2045" t="s">
+        <v>2021</v>
+      </c>
+      <c r="D2045" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2046" spans="1:4">
+      <c r="A2046" s="4" t="s">
+        <v>2020</v>
+      </c>
+      <c r="B2046" s="11" t="s">
+        <v>994</v>
+      </c>
+      <c r="C2046" t="s">
+        <v>995</v>
+      </c>
+      <c r="D2046" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2047" spans="1:4">
+      <c r="A2047" s="4" t="s">
+        <v>2020</v>
+      </c>
+      <c r="B2047" s="11" t="s">
+        <v>1115</v>
+      </c>
+      <c r="C2047" t="s">
+        <v>1116</v>
+      </c>
+      <c r="D2047" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2048" spans="1:4">
+      <c r="A2048" s="4" t="s">
+        <v>2020</v>
+      </c>
+      <c r="B2048" s="11" t="s">
+        <v>1770</v>
+      </c>
+      <c r="C2048" t="s">
+        <v>1771</v>
+      </c>
+      <c r="D2048" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2049" spans="1:4">
+      <c r="A2049" s="4" t="s">
+        <v>2020</v>
+      </c>
+      <c r="B2049" s="7">
+        <v>300394</v>
+      </c>
+      <c r="C2049" t="s">
+        <v>2022</v>
+      </c>
+      <c r="D2049" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2050" spans="1:4">
+      <c r="A2050" s="4" t="s">
+        <v>2020</v>
+      </c>
+      <c r="B2050" s="7">
+        <v>300502</v>
+      </c>
+      <c r="C2050" t="s">
+        <v>2023</v>
+      </c>
+      <c r="D2050" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2051" spans="1:4">
+      <c r="A2051" s="4" t="s">
+        <v>2020</v>
+      </c>
+      <c r="B2051" s="7">
+        <v>600066</v>
+      </c>
+      <c r="C2051" t="s">
+        <v>759</v>
+      </c>
+      <c r="D2051" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2052" spans="1:4">
+      <c r="A2052" s="4" t="s">
+        <v>2020</v>
+      </c>
+      <c r="B2052" s="7">
+        <v>600160</v>
+      </c>
+      <c r="C2052" t="s">
+        <v>766</v>
+      </c>
+      <c r="D2052" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2053" spans="1:4">
+      <c r="A2053" s="4" t="s">
+        <v>2020</v>
+      </c>
+      <c r="B2053" s="7">
+        <v>600377</v>
+      </c>
+      <c r="C2053" t="s">
+        <v>433</v>
+      </c>
+      <c r="D2053" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2054" spans="1:4">
+      <c r="A2054" s="4" t="s">
+        <v>2020</v>
+      </c>
+      <c r="B2054" s="7">
+        <v>600482</v>
+      </c>
+      <c r="C2054" t="s">
+        <v>1522</v>
+      </c>
+      <c r="D2054" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2055" spans="1:4">
+      <c r="A2055" s="4" t="s">
+        <v>2020</v>
+      </c>
+      <c r="B2055" s="7">
+        <v>601127</v>
+      </c>
+      <c r="C2055" t="s">
+        <v>2024</v>
+      </c>
+      <c r="D2055" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2056" spans="1:4">
+      <c r="A2056" s="4" t="s">
+        <v>2020</v>
+      </c>
+      <c r="B2056" s="7">
+        <v>601136</v>
+      </c>
+      <c r="C2056" t="s">
+        <v>2025</v>
+      </c>
+      <c r="D2056" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2057" spans="1:4">
+      <c r="A2057" s="4" t="s">
+        <v>2020</v>
+      </c>
+      <c r="B2057" s="7">
+        <v>688169</v>
+      </c>
+      <c r="C2057" t="s">
+        <v>1883</v>
+      </c>
+      <c r="D2057" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2058" spans="1:4">
+      <c r="A2058" s="4" t="s">
+        <v>2020</v>
+      </c>
+      <c r="B2058" s="7">
+        <v>688472</v>
+      </c>
+      <c r="C2058" t="s">
+        <v>2026</v>
+      </c>
+      <c r="D2058" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2059" spans="1:4">
+      <c r="A2059" s="4" t="s">
+        <v>2020</v>
+      </c>
+      <c r="B2059" s="7">
+        <v>688506</v>
+      </c>
+      <c r="C2059" t="s">
+        <v>2027</v>
+      </c>
+      <c r="D2059" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2060" spans="1:4">
+      <c r="A2060" s="4" t="s">
+        <v>2020</v>
+      </c>
+      <c r="B2060" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="C2060" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="D2060" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="2061" spans="1:4">
+      <c r="A2061" s="4" t="s">
+        <v>2020</v>
+      </c>
+      <c r="B2061" s="11" t="s">
+        <v>1323</v>
+      </c>
+      <c r="C2061" s="7" t="s">
+        <v>1324</v>
+      </c>
+      <c r="D2061" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="2062" spans="1:4">
+      <c r="A2062" s="4" t="s">
+        <v>2020</v>
+      </c>
+      <c r="B2062" s="11" t="s">
+        <v>1193</v>
+      </c>
+      <c r="C2062" s="7" t="s">
+        <v>1194</v>
+      </c>
+      <c r="D2062" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="2063" spans="1:4">
+      <c r="A2063" s="4" t="s">
+        <v>2020</v>
+      </c>
+      <c r="B2063" s="11" t="s">
+        <v>1810</v>
+      </c>
+      <c r="C2063" s="7" t="s">
+        <v>1811</v>
+      </c>
+      <c r="D2063" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="2064" spans="1:4">
+      <c r="A2064" s="4" t="s">
+        <v>2020</v>
+      </c>
+      <c r="B2064" s="11" t="s">
+        <v>1550</v>
+      </c>
+      <c r="C2064" s="7" t="s">
+        <v>1551</v>
+      </c>
+      <c r="D2064" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="2065" spans="1:4">
+      <c r="A2065" s="4" t="s">
+        <v>2020</v>
+      </c>
+      <c r="B2065" s="7">
+        <v>300142</v>
+      </c>
+      <c r="C2065" s="7" t="s">
+        <v>1683</v>
+      </c>
+      <c r="D2065" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="2066" spans="1:4">
+      <c r="A2066" s="4" t="s">
+        <v>2020</v>
+      </c>
+      <c r="B2066" s="7">
+        <v>300223</v>
+      </c>
+      <c r="C2066" s="7" t="s">
+        <v>1950</v>
+      </c>
+      <c r="D2066" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="2067" spans="1:4">
+      <c r="A2067" s="4" t="s">
+        <v>2020</v>
+      </c>
+      <c r="B2067" s="7">
+        <v>300454</v>
+      </c>
+      <c r="C2067" s="7" t="s">
+        <v>1952</v>
+      </c>
+      <c r="D2067" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="2068" spans="1:4">
+      <c r="A2068" s="4" t="s">
+        <v>2020</v>
+      </c>
+      <c r="B2068" s="7">
+        <v>300496</v>
+      </c>
+      <c r="C2068" s="7" t="s">
+        <v>1954</v>
+      </c>
+      <c r="D2068" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="2069" spans="1:4">
+      <c r="A2069" s="4" t="s">
+        <v>2020</v>
+      </c>
+      <c r="B2069" s="7">
+        <v>300751</v>
+      </c>
+      <c r="C2069" s="7" t="s">
+        <v>1958</v>
+      </c>
+      <c r="D2069" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="2070" spans="1:4">
+      <c r="A2070" s="4" t="s">
+        <v>2020</v>
+      </c>
+      <c r="B2070" s="7">
+        <v>300919</v>
+      </c>
+      <c r="C2070" s="7" t="s">
+        <v>1962</v>
+      </c>
+      <c r="D2070" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="2071" spans="1:4">
+      <c r="A2071" s="4" t="s">
+        <v>2020</v>
+      </c>
+      <c r="B2071" s="7">
+        <v>300957</v>
+      </c>
+      <c r="C2071" s="7" t="s">
+        <v>1964</v>
+      </c>
+      <c r="D2071" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="2072" spans="1:4">
+      <c r="A2072" s="4" t="s">
+        <v>2020</v>
+      </c>
+      <c r="B2072" s="7">
+        <v>600132</v>
+      </c>
+      <c r="C2072" s="7" t="s">
+        <v>681</v>
+      </c>
+      <c r="D2072" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="2073" spans="1:4">
+      <c r="A2073" s="4" t="s">
+        <v>2020</v>
+      </c>
+      <c r="B2073" s="7">
+        <v>600732</v>
+      </c>
+      <c r="C2073" s="7" t="s">
+        <v>1998</v>
+      </c>
+      <c r="D2073" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="2074" spans="1:4">
+      <c r="A2074" s="4" t="s">
+        <v>2020</v>
+      </c>
+      <c r="B2074" s="7">
+        <v>603899</v>
+      </c>
+      <c r="C2074" s="7" t="s">
+        <v>2028</v>
+      </c>
+      <c r="D2074" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="2075" spans="1:4">
+      <c r="A2075" s="4" t="s">
+        <v>2020</v>
+      </c>
+      <c r="B2075" s="7">
+        <v>688363</v>
+      </c>
+      <c r="C2075" s="7" t="s">
+        <v>1885</v>
+      </c>
+      <c r="D2075" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="2076" spans="1:4">
+      <c r="A2076" s="4" t="s">
+        <v>2029</v>
+      </c>
+      <c r="B2076" s="7">
+        <v>601058</v>
+      </c>
+      <c r="C2076" t="s">
+        <v>2030</v>
+      </c>
+      <c r="D2076" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2077" spans="1:4">
+      <c r="A2077" s="4" t="s">
+        <v>2029</v>
+      </c>
+      <c r="B2077" s="7">
+        <v>600837</v>
+      </c>
+      <c r="C2077" t="s">
+        <v>2031</v>
+      </c>
+      <c r="D2077" t="s">
+        <v>607</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="A1:D2019" etc:filterBottomFollowUsedRange="0">
-    <sortState ref="A1:D2019">
+  <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="A1:D2043" etc:filterBottomFollowUsedRange="0">
+    <sortState ref="A1:D2043">
       <sortCondition ref="A2"/>
     </sortState>
     <extLst/>
@@ -35748,7 +36260,7 @@
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter/>
   <ignoredErrors>
-    <ignoredError sqref="B1983:B1986 B1974:B1975 B1992:B1993 B2006:B2010" numberStoredAsText="1"/>
+    <ignoredError sqref="B2060:B2064 B2044:B2048 B2006:B2010 B1992:B1993 B1974:B1975 B1983:B1986" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>